<commit_message>
Integrated facial recognition in login
</commit_message>
<xml_diff>
--- a/backend/downloads/attendance_reports/AttendanceReport.xlsx
+++ b/backend/downloads/attendance_reports/AttendanceReport.xlsx
@@ -491,7 +491,7 @@
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>5:40 PM</t>
+          <t>4:24 PM</t>
         </is>
       </c>
     </row>
@@ -516,7 +516,7 @@
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>4:24 PM</t>
+          <t>5:40 PM</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Finished notifications for admins, and added a button for handling issues within notifications
</commit_message>
<xml_diff>
--- a/backend/downloads/attendance_reports/AttendanceReport.xlsx
+++ b/backend/downloads/attendance_reports/AttendanceReport.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,62 +486,12 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>Sun, Sep 24, 2023</t>
+          <t>Thu, Sep 28, 2023</t>
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>4:24 PM</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>Ahmed Mahmoud</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>Cairo, Egypt</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="inlineStr">
-        <is>
-          <t>Sun, Sep 24, 2023</t>
-        </is>
-      </c>
-      <c r="E3" s="2" t="inlineStr">
-        <is>
-          <t>5:40 PM</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>Ahmed Mahmoud</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>Cairo, Egypt</t>
-        </is>
-      </c>
-      <c r="D4" s="2" t="inlineStr">
-        <is>
-          <t>Mon, Sep 25, 2023</t>
-        </is>
-      </c>
-      <c r="E4" s="2" t="inlineStr">
-        <is>
-          <t>3:33 PM</t>
+          <t>9:41 PM</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Finished departments page, added skeletons, fixed issues with table in attendances
</commit_message>
<xml_diff>
--- a/backend/downloads/attendance_reports/AttendanceReport.xlsx
+++ b/backend/downloads/attendance_reports/AttendanceReport.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,6 +495,81 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>Ahmed Mahmoud</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>Cairo, Egypt</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>Fri, Sep 29, 2023</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>3:59 AM</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>Farah Mahmoud</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>Cairo, Egypt</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>Fri, Sep 29, 2023</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>1:02 AM</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>Farah Mahmoud</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>Cairo, Egypt</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>Fri, Sep 29, 2023</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>4:00 AM</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>